<commit_message>
Added more command line parameters and docu
</commit_message>
<xml_diff>
--- a/data/CLL-DB-data-aligned_14_seqs.xlsx
+++ b/data/CLL-DB-data-aligned_14_seqs.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L15"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,47 +451,22 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>aa sequence aligned</t>
+          <t>Predicted Cluster for h = 0.12609303928911686</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Predicted Cluster for h = 0.09867135528475046</t>
+          <t>Predicted Cluster for h = 0.20445840433239937</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Predicted Cluster for h = 0.14600748103111982</t>
+          <t>Predicted Cluster for h = 0.24568521697074175</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Predicted Cluster for h = 0.19810745352879167</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Predicted Cluster for h = 0.2291366928257048</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Predicted Cluster for h = 0.23818379221484065</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>Predicted Cluster for h = 0.24838136555626988</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>Predicted Cluster for h = 0.2636352088302374</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>Predicted Cluster for h = 0.282840589992702</t>
+          <t>Predicted Cluster for h = 0.2750881714746356</t>
         </is>
       </c>
     </row>
@@ -511,33 +486,18 @@
           <t>IGHV1-3</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>QVQLVQSGA.EVKKPGASVKVSCKASGYTF....TSYAMHWVRQAPGQRLEWMGWINAG..NGNTKYSQKFQ.GRVTITRDTSASTAYMELSSLRSEDTAVYYCAREQWLVRVYFDYWGQGTLVTVSS</t>
-        </is>
+      <c r="D2" t="n">
+        <v>3</v>
       </c>
       <c r="E2" t="n">
-        <v>1</v>
-      </c>
-      <c r="F2" t="n">
-        <v>5</v>
-      </c>
-      <c r="G2" t="n">
-        <v>140</v>
-      </c>
-      <c r="H2" t="n">
-        <v>135</v>
-      </c>
-      <c r="I2" t="n">
-        <v>5</v>
-      </c>
-      <c r="J2" t="n">
-        <v>13</v>
-      </c>
-      <c r="K2" t="n">
-        <v>41</v>
-      </c>
-      <c r="L2" t="inlineStr">
+        <v>4</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
         <is>
           <t>no</t>
         </is>
@@ -559,33 +519,18 @@
           <t>IGHV1-2</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>QVQLVQSGA.EVKKPGASVKVSCKASGYTF....TGYYMHWVRQAPGQGLEWMGWINPN..SGGTNYAQKFQ.GRVTMTRDTSISTAYMELSRLRSDDTAVYYCAREQWLPTNYFDYWGQGTLVTVSS</t>
-        </is>
+      <c r="D3" t="n">
+        <v>3</v>
       </c>
       <c r="E3" t="n">
-        <v>1</v>
-      </c>
-      <c r="F3" t="n">
-        <v>5</v>
-      </c>
-      <c r="G3" t="n">
-        <v>140</v>
-      </c>
-      <c r="H3" t="n">
-        <v>145</v>
-      </c>
-      <c r="I3" t="n">
-        <v>5</v>
-      </c>
-      <c r="J3" t="n">
-        <v>13</v>
-      </c>
-      <c r="K3" t="n">
-        <v>41</v>
-      </c>
-      <c r="L3" t="inlineStr">
+        <v>4</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
         <is>
           <t>no</t>
         </is>
@@ -607,35 +552,18 @@
           <t>IGHV1-3</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>QVQLVQSGA.EVKKPGASVKFSCKASGYTF....TSYAMHWVRQAPGQRLEWMGWINAG..NGNTKYSQKFQ.GRVTITRDTSASTAYMELSSLRSEDTAVYYCAREQWLSLGDYFDYWGQGTLVTVSS</t>
-        </is>
+      <c r="D4" t="n">
+        <v>3</v>
       </c>
       <c r="E4" t="n">
-        <v>1</v>
-      </c>
-      <c r="F4" t="n">
-        <v>5</v>
-      </c>
-      <c r="G4" t="n">
-        <v>140</v>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
-      <c r="I4" t="n">
-        <v>5</v>
-      </c>
-      <c r="J4" t="n">
-        <v>13</v>
-      </c>
-      <c r="K4" t="n">
-        <v>41</v>
-      </c>
-      <c r="L4" t="inlineStr">
+        <v>3</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
         <is>
           <t>no</t>
         </is>
@@ -657,35 +585,18 @@
           <t>IGHV1-2</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>QVQLVQSGA.EVKKPGASVKVSCKASGYTF....TGYYMHWVRQAPGQGLEWMGWINPN..SGGTNYAQKFQ.GRVTMTRDTSISTAYMELSRLRSDDTAVYYCARSQWLALVYYFDYWGQGTLVT</t>
-        </is>
+      <c r="D5" t="n">
+        <v>3</v>
       </c>
       <c r="E5" t="n">
-        <v>1</v>
-      </c>
-      <c r="F5" t="n">
-        <v>5</v>
-      </c>
-      <c r="G5" t="n">
-        <v>140</v>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
-      <c r="I5" t="n">
-        <v>5</v>
-      </c>
-      <c r="J5" t="n">
-        <v>13</v>
-      </c>
-      <c r="K5" t="n">
-        <v>41</v>
-      </c>
-      <c r="L5" t="inlineStr">
+        <v>3</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
         <is>
           <t>no</t>
         </is>
@@ -707,35 +618,18 @@
           <t>IGHV4-34</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>QEHLQQWGA.GLLKPSETLSLTCGVYGGSF....SGFYWSWIRQPPGKGLEWIGEINHS...GSTKYNPSFK.SRVTISVDTAKNQFSLRVRSVTAADTAVYYCARGYPEVPTTRRYYYYGMELWGQGTTVTVSS</t>
-        </is>
+      <c r="D6" t="n">
+        <v>1</v>
       </c>
       <c r="E6" t="n">
         <v>1</v>
       </c>
-      <c r="F6" t="n">
-        <v>4</v>
-      </c>
-      <c r="G6" t="n">
-        <v>116</v>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
-      <c r="I6" t="n">
-        <v>4</v>
-      </c>
-      <c r="J6" t="n">
-        <v>6</v>
-      </c>
-      <c r="K6" t="n">
-        <v>22</v>
-      </c>
-      <c r="L6" t="inlineStr">
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
         <is>
           <t>no</t>
         </is>
@@ -757,35 +651,18 @@
           <t>IGHV4-34</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>QVQLQQWGA.GLLKPSETLSLTCAVYGESF....SGFYWTWIRQPPGKGLEYIGDITHT...GSTSYNPSLK.SRVTISVDSSKNQFSLKLTSVTAADTAVYYCARGWPDTAVTKRYYYYGMEVWGQGTTVTVSP</t>
-        </is>
+      <c r="D7" t="n">
+        <v>1</v>
       </c>
       <c r="E7" t="n">
         <v>1</v>
       </c>
-      <c r="F7" t="n">
-        <v>4</v>
-      </c>
-      <c r="G7" t="n">
-        <v>116</v>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
-      <c r="I7" t="n">
-        <v>4</v>
-      </c>
-      <c r="J7" t="n">
-        <v>6</v>
-      </c>
-      <c r="K7" t="n">
-        <v>22</v>
-      </c>
-      <c r="L7" t="inlineStr">
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
         <is>
           <t>no</t>
         </is>
@@ -807,33 +684,16 @@
           <t>IGHV3-21</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>EVQLVESGG.GLVKPGGSLRLSCAASGFTF....SSYSMNWVRQAPGKGLEWVSSISSS..SNYIYYADSVK.GRFTISRDNAKNSLYLQMNSLRAEDTAVYYCARDESAYDSWGQGTLVTVSS</t>
-        </is>
+      <c r="D8" t="n">
+        <v>2</v>
       </c>
       <c r="E8" t="n">
+        <v>2</v>
+      </c>
+      <c r="F8" t="n">
         <v>1</v>
       </c>
-      <c r="F8" t="n">
-        <v>5</v>
-      </c>
-      <c r="G8" t="n">
-        <v>151</v>
-      </c>
-      <c r="H8" t="n">
-        <v>106</v>
-      </c>
-      <c r="I8" t="n">
-        <v>5</v>
-      </c>
-      <c r="J8" t="n">
-        <v>10</v>
-      </c>
-      <c r="K8" t="n">
-        <v>35</v>
-      </c>
-      <c r="L8" t="inlineStr">
+      <c r="G8" t="inlineStr">
         <is>
           <t>no</t>
         </is>
@@ -855,33 +715,16 @@
           <t>IGHV3-21</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>EVQLVESGG.GLGKPGGSLRLSCGASGFTF....SSYSMNWVRQAPGKGLEWVSSISSS..SSYINYADSVK.GRFTISRDNAKNSLYLQMNSLRVEDTAVYYCARDANCMDVWGQGTTVTVSS</t>
-        </is>
+      <c r="D9" t="n">
+        <v>2</v>
       </c>
       <c r="E9" t="n">
+        <v>2</v>
+      </c>
+      <c r="F9" t="n">
         <v>1</v>
       </c>
-      <c r="F9" t="n">
-        <v>5</v>
-      </c>
-      <c r="G9" t="n">
-        <v>151</v>
-      </c>
-      <c r="H9" t="n">
-        <v>94</v>
-      </c>
-      <c r="I9" t="n">
-        <v>5</v>
-      </c>
-      <c r="J9" t="n">
-        <v>10</v>
-      </c>
-      <c r="K9" t="n">
-        <v>35</v>
-      </c>
-      <c r="L9" t="inlineStr">
+      <c r="G9" t="inlineStr">
         <is>
           <t>no</t>
         </is>
@@ -903,33 +746,18 @@
           <t>IGHV3-48</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>EVQLVESGG.GLVQPGGSLRLSCAASGFTF....SSYNMNWVRQAPGKGLEWVSHISSS..SSTIYYADSVK.GRFTISRDNAKNSLYLQMNSLRDEDTAVYYCARDGEGPTVWGQGTLVTVSS</t>
-        </is>
+      <c r="D10" t="n">
+        <v>2</v>
       </c>
       <c r="E10" t="n">
-        <v>1</v>
-      </c>
-      <c r="F10" t="n">
-        <v>5</v>
-      </c>
-      <c r="G10" t="n">
-        <v>151</v>
-      </c>
-      <c r="H10" t="n">
-        <v>106</v>
-      </c>
-      <c r="I10" t="n">
-        <v>5</v>
-      </c>
-      <c r="J10" t="n">
-        <v>10</v>
-      </c>
-      <c r="K10" t="n">
-        <v>35</v>
-      </c>
-      <c r="L10" t="inlineStr">
+        <v>2</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
         <is>
           <t>no</t>
         </is>
@@ -953,45 +781,20 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>QVQLQQWGA.GLLKPSETLSLTCAVYDGSF....SGYYWSWIRQPPGKGLEWIGEINHS...GSTNYNPSLK.SRVTISADTSKSQFSVRLSSVTAADTAVYYCAGRFYCSGATCYSEAYHYYYGMDVWGQG</t>
+          <t>no</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Not Found</t>
+          <t>no</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Not Found</t>
+          <t>no</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="L11" t="inlineStr">
         <is>
           <t>no</t>
         </is>
@@ -1015,45 +818,20 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>QVHLQQWGA.GLLKPSETLSLTCAVYGGSF....SDYYWTWIRQPPGKGLEWIAGINHI...GIINWNLSLK.TRVTVSIDTFEHQFSLQLRSVTAADAAVYYCARRGIYSDHNLNDAFDLWGQGTMVTVSS</t>
+          <t>no</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Not Found</t>
+          <t>no</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Not Found</t>
+          <t>no</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="L12" t="inlineStr">
         <is>
           <t>no</t>
         </is>
@@ -1077,45 +855,20 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>EVHLVESGG.GLVKPGGSLRLSCVASGFAF....SDYTINWVRQAPGSGLEWVSCISSS..SDYIYYADSVR.GRFTLSRANAKNSVYLQMNSLRVEDSAVYYCSRDNCSNTNCNKGAEYYYYYGMDAWGQGTTVTVSS</t>
+          <t>no</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Not Found</t>
+          <t>no</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Not Found</t>
+          <t>no</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="K13" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="L13" t="inlineStr">
         <is>
           <t>no</t>
         </is>
@@ -1139,45 +892,20 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>QVQLVQSGA.EVKKPGASVKVSCKASGYTF....TGYYMHWVRQAPGQGLEWMGWINPN..SGGTNYAQKFQ.GRVTMTRDTSISTAYMELSRLRSDDTAVYYCARDGISGYCSSASCWPSGFHVDPWGQGTLVT</t>
+          <t>no</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Not Found</t>
+          <t>no</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Not Found</t>
+          <t>no</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="J14" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="K14" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="L14" t="inlineStr">
         <is>
           <t>no</t>
         </is>
@@ -1201,45 +929,20 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>QVQLVQSGA.EVKKPGASVMISCKASGYIF....TFYSMHWVRQAPGQRLEWMGWIAGA..DDNKKYSQKFQ.DRLTITRDTSASTVYMELRGLRSEDTAVYYCGRGLRHLEGLLYGEDAFDFWGQGTIVT</t>
+          <t>no</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Not Found</t>
+          <t>no</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Not Found</t>
+          <t>no</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="J15" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="K15" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="L15" t="inlineStr">
         <is>
           <t>no</t>
         </is>

</xml_diff>